<commit_message>
Added Read_Me, restructured settings file
</commit_message>
<xml_diff>
--- a/0_0_Data/0_Forecast_Inputs/1_ifo_quarterly_gdp/ifo_Konjunkturprognose_Quartalsdaten_Archiv_H25.xlsx
+++ b/0_0_Data/0_Forecast_Inputs/1_ifo_quarterly_gdp/ifo_Konjunkturprognose_Quartalsdaten_Archiv_H25.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dfbe04e23282f0d1/Desktop/ifo/Konjunkturprognose Evaluierung/ifo Forecast Evaluation Workfolder/0_0_Data/0_Forecast_Inputs/1_ifo_quarterly_gdp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A04D1F-2272-4A71-9A17-C9FD01CE6BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{74A04D1F-2272-4A71-9A17-C9FD01CE6BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{750D1199-FF2C-4417-BD74-DC4BDD247909}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="934" firstSheet="21" activeTab="46" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="934" firstSheet="22" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Read me" sheetId="48" r:id="rId1"/>
@@ -2243,6 +2243,9 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2263,9 +2266,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -4158,40 +4158,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="175" t="s">
+      <c r="A1" s="176" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="175"/>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
-      <c r="G1" s="175"/>
-      <c r="H1" s="175"/>
-      <c r="I1" s="175"/>
-      <c r="J1" s="175"/>
-      <c r="K1" s="175"/>
-      <c r="L1" s="175"/>
-      <c r="M1" s="175"/>
-      <c r="N1" s="175"/>
+      <c r="B1" s="176"/>
+      <c r="C1" s="176"/>
+      <c r="D1" s="176"/>
+      <c r="E1" s="176"/>
+      <c r="F1" s="176"/>
+      <c r="G1" s="176"/>
+      <c r="H1" s="176"/>
+      <c r="I1" s="176"/>
+      <c r="J1" s="176"/>
+      <c r="K1" s="176"/>
+      <c r="L1" s="176"/>
+      <c r="M1" s="176"/>
+      <c r="N1" s="176"/>
     </row>
     <row r="2" spans="1:14" ht="13" x14ac:dyDescent="0.25">
-      <c r="A2" s="176" t="s">
+      <c r="A2" s="177" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="176"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="176"/>
-      <c r="F2" s="176"/>
-      <c r="G2" s="176"/>
-      <c r="H2" s="176"/>
-      <c r="I2" s="176"/>
-      <c r="J2" s="176"/>
-      <c r="K2" s="176"/>
-      <c r="L2" s="176"/>
-      <c r="M2" s="176"/>
-      <c r="N2" s="176"/>
+      <c r="B2" s="177"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="177"/>
+      <c r="I2" s="177"/>
+      <c r="J2" s="177"/>
+      <c r="K2" s="177"/>
+      <c r="L2" s="177"/>
+      <c r="M2" s="177"/>
+      <c r="N2" s="177"/>
     </row>
     <row r="3" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A3" s="82"/>
@@ -4199,21 +4199,21 @@
       <c r="C3" s="192">
         <v>2022</v>
       </c>
-      <c r="D3" s="178"/>
-      <c r="E3" s="178"/>
-      <c r="F3" s="178"/>
-      <c r="G3" s="179">
+      <c r="D3" s="179"/>
+      <c r="E3" s="179"/>
+      <c r="F3" s="179"/>
+      <c r="G3" s="180">
         <v>2023</v>
       </c>
-      <c r="H3" s="180"/>
-      <c r="I3" s="180"/>
-      <c r="J3" s="181"/>
-      <c r="K3" s="179">
+      <c r="H3" s="181"/>
+      <c r="I3" s="181"/>
+      <c r="J3" s="182"/>
+      <c r="K3" s="180">
         <v>2024</v>
       </c>
-      <c r="L3" s="180"/>
-      <c r="M3" s="180"/>
-      <c r="N3" s="180"/>
+      <c r="L3" s="181"/>
+      <c r="M3" s="181"/>
+      <c r="N3" s="181"/>
     </row>
     <row r="4" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A4" s="84"/>
@@ -4718,22 +4718,22 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="182" t="s">
+      <c r="A16" s="175" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="182"/>
-      <c r="C16" s="182"/>
-      <c r="D16" s="182"/>
-      <c r="E16" s="182"/>
-      <c r="F16" s="182"/>
-      <c r="G16" s="182"/>
-      <c r="H16" s="182"/>
-      <c r="I16" s="182"/>
-      <c r="J16" s="182"/>
-      <c r="K16" s="182"/>
-      <c r="L16" s="182"/>
-      <c r="M16" s="182"/>
-      <c r="N16" s="182"/>
+      <c r="B16" s="175"/>
+      <c r="C16" s="175"/>
+      <c r="D16" s="175"/>
+      <c r="E16" s="175"/>
+      <c r="F16" s="175"/>
+      <c r="G16" s="175"/>
+      <c r="H16" s="175"/>
+      <c r="I16" s="175"/>
+      <c r="J16" s="175"/>
+      <c r="K16" s="175"/>
+      <c r="L16" s="175"/>
+      <c r="M16" s="175"/>
+      <c r="N16" s="175"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="104" t="s">
@@ -4782,40 +4782,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="175" t="s">
+      <c r="A1" s="176" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="175"/>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
-      <c r="G1" s="175"/>
-      <c r="H1" s="175"/>
-      <c r="I1" s="175"/>
-      <c r="J1" s="175"/>
-      <c r="K1" s="175"/>
-      <c r="L1" s="175"/>
-      <c r="M1" s="175"/>
-      <c r="N1" s="175"/>
+      <c r="B1" s="176"/>
+      <c r="C1" s="176"/>
+      <c r="D1" s="176"/>
+      <c r="E1" s="176"/>
+      <c r="F1" s="176"/>
+      <c r="G1" s="176"/>
+      <c r="H1" s="176"/>
+      <c r="I1" s="176"/>
+      <c r="J1" s="176"/>
+      <c r="K1" s="176"/>
+      <c r="L1" s="176"/>
+      <c r="M1" s="176"/>
+      <c r="N1" s="176"/>
     </row>
     <row r="2" spans="1:14" ht="13" x14ac:dyDescent="0.25">
-      <c r="A2" s="176" t="s">
+      <c r="A2" s="177" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="176"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="176"/>
-      <c r="F2" s="176"/>
-      <c r="G2" s="176"/>
-      <c r="H2" s="176"/>
-      <c r="I2" s="176"/>
-      <c r="J2" s="176"/>
-      <c r="K2" s="176"/>
-      <c r="L2" s="176"/>
-      <c r="M2" s="176"/>
-      <c r="N2" s="176"/>
+      <c r="B2" s="177"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="177"/>
+      <c r="I2" s="177"/>
+      <c r="J2" s="177"/>
+      <c r="K2" s="177"/>
+      <c r="L2" s="177"/>
+      <c r="M2" s="177"/>
+      <c r="N2" s="177"/>
     </row>
     <row r="3" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A3" s="82"/>
@@ -4823,21 +4823,21 @@
       <c r="C3" s="192">
         <v>2022</v>
       </c>
-      <c r="D3" s="178"/>
-      <c r="E3" s="178"/>
-      <c r="F3" s="178"/>
-      <c r="G3" s="179">
+      <c r="D3" s="179"/>
+      <c r="E3" s="179"/>
+      <c r="F3" s="179"/>
+      <c r="G3" s="180">
         <v>2023</v>
       </c>
-      <c r="H3" s="180"/>
-      <c r="I3" s="180"/>
-      <c r="J3" s="181"/>
-      <c r="K3" s="179">
+      <c r="H3" s="181"/>
+      <c r="I3" s="181"/>
+      <c r="J3" s="182"/>
+      <c r="K3" s="180">
         <v>2024</v>
       </c>
-      <c r="L3" s="180"/>
-      <c r="M3" s="180"/>
-      <c r="N3" s="180"/>
+      <c r="L3" s="181"/>
+      <c r="M3" s="181"/>
+      <c r="N3" s="181"/>
     </row>
     <row r="4" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A4" s="84"/>
@@ -5342,22 +5342,22 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="182" t="s">
+      <c r="A16" s="175" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="182"/>
-      <c r="C16" s="182"/>
-      <c r="D16" s="182"/>
-      <c r="E16" s="182"/>
-      <c r="F16" s="182"/>
-      <c r="G16" s="182"/>
-      <c r="H16" s="182"/>
-      <c r="I16" s="182"/>
-      <c r="J16" s="182"/>
-      <c r="K16" s="182"/>
-      <c r="L16" s="182"/>
-      <c r="M16" s="182"/>
-      <c r="N16" s="182"/>
+      <c r="B16" s="175"/>
+      <c r="C16" s="175"/>
+      <c r="D16" s="175"/>
+      <c r="E16" s="175"/>
+      <c r="F16" s="175"/>
+      <c r="G16" s="175"/>
+      <c r="H16" s="175"/>
+      <c r="I16" s="175"/>
+      <c r="J16" s="175"/>
+      <c r="K16" s="175"/>
+      <c r="L16" s="175"/>
+      <c r="M16" s="175"/>
+      <c r="N16" s="175"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="104" t="s">
@@ -5406,40 +5406,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="175" t="s">
+      <c r="A1" s="176" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="175"/>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
-      <c r="G1" s="175"/>
-      <c r="H1" s="175"/>
-      <c r="I1" s="175"/>
-      <c r="J1" s="175"/>
-      <c r="K1" s="175"/>
-      <c r="L1" s="175"/>
-      <c r="M1" s="175"/>
-      <c r="N1" s="175"/>
+      <c r="B1" s="176"/>
+      <c r="C1" s="176"/>
+      <c r="D1" s="176"/>
+      <c r="E1" s="176"/>
+      <c r="F1" s="176"/>
+      <c r="G1" s="176"/>
+      <c r="H1" s="176"/>
+      <c r="I1" s="176"/>
+      <c r="J1" s="176"/>
+      <c r="K1" s="176"/>
+      <c r="L1" s="176"/>
+      <c r="M1" s="176"/>
+      <c r="N1" s="176"/>
     </row>
     <row r="2" spans="1:14" ht="13" x14ac:dyDescent="0.25">
-      <c r="A2" s="176" t="s">
+      <c r="A2" s="177" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="176"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="176"/>
-      <c r="F2" s="176"/>
-      <c r="G2" s="176"/>
-      <c r="H2" s="176"/>
-      <c r="I2" s="176"/>
-      <c r="J2" s="176"/>
-      <c r="K2" s="176"/>
-      <c r="L2" s="176"/>
-      <c r="M2" s="176"/>
-      <c r="N2" s="176"/>
+      <c r="B2" s="177"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="177"/>
+      <c r="I2" s="177"/>
+      <c r="J2" s="177"/>
+      <c r="K2" s="177"/>
+      <c r="L2" s="177"/>
+      <c r="M2" s="177"/>
+      <c r="N2" s="177"/>
     </row>
     <row r="3" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A3" s="82"/>
@@ -5447,21 +5447,21 @@
       <c r="C3" s="192">
         <v>2022</v>
       </c>
-      <c r="D3" s="178"/>
-      <c r="E3" s="178"/>
-      <c r="F3" s="178"/>
-      <c r="G3" s="179">
+      <c r="D3" s="179"/>
+      <c r="E3" s="179"/>
+      <c r="F3" s="179"/>
+      <c r="G3" s="180">
         <v>2023</v>
       </c>
-      <c r="H3" s="180"/>
-      <c r="I3" s="180"/>
-      <c r="J3" s="181"/>
-      <c r="K3" s="179">
+      <c r="H3" s="181"/>
+      <c r="I3" s="181"/>
+      <c r="J3" s="182"/>
+      <c r="K3" s="180">
         <v>2024</v>
       </c>
-      <c r="L3" s="180"/>
-      <c r="M3" s="180"/>
-      <c r="N3" s="180"/>
+      <c r="L3" s="181"/>
+      <c r="M3" s="181"/>
+      <c r="N3" s="181"/>
     </row>
     <row r="4" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A4" s="84"/>
@@ -5966,22 +5966,22 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="182" t="s">
+      <c r="A16" s="175" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="182"/>
-      <c r="C16" s="182"/>
-      <c r="D16" s="182"/>
-      <c r="E16" s="182"/>
-      <c r="F16" s="182"/>
-      <c r="G16" s="182"/>
-      <c r="H16" s="182"/>
-      <c r="I16" s="182"/>
-      <c r="J16" s="182"/>
-      <c r="K16" s="182"/>
-      <c r="L16" s="182"/>
-      <c r="M16" s="182"/>
-      <c r="N16" s="182"/>
+      <c r="B16" s="175"/>
+      <c r="C16" s="175"/>
+      <c r="D16" s="175"/>
+      <c r="E16" s="175"/>
+      <c r="F16" s="175"/>
+      <c r="G16" s="175"/>
+      <c r="H16" s="175"/>
+      <c r="I16" s="175"/>
+      <c r="J16" s="175"/>
+      <c r="K16" s="175"/>
+      <c r="L16" s="175"/>
+      <c r="M16" s="175"/>
+      <c r="N16" s="175"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="104" t="s">
@@ -6030,40 +6030,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="175" t="s">
+      <c r="A1" s="176" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="175"/>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
-      <c r="G1" s="175"/>
-      <c r="H1" s="175"/>
-      <c r="I1" s="175"/>
-      <c r="J1" s="175"/>
-      <c r="K1" s="175"/>
-      <c r="L1" s="175"/>
-      <c r="M1" s="175"/>
-      <c r="N1" s="175"/>
+      <c r="B1" s="176"/>
+      <c r="C1" s="176"/>
+      <c r="D1" s="176"/>
+      <c r="E1" s="176"/>
+      <c r="F1" s="176"/>
+      <c r="G1" s="176"/>
+      <c r="H1" s="176"/>
+      <c r="I1" s="176"/>
+      <c r="J1" s="176"/>
+      <c r="K1" s="176"/>
+      <c r="L1" s="176"/>
+      <c r="M1" s="176"/>
+      <c r="N1" s="176"/>
     </row>
     <row r="2" spans="1:14" ht="13" x14ac:dyDescent="0.25">
-      <c r="A2" s="176" t="s">
+      <c r="A2" s="177" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="176"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="176"/>
-      <c r="F2" s="176"/>
-      <c r="G2" s="176"/>
-      <c r="H2" s="176"/>
-      <c r="I2" s="176"/>
-      <c r="J2" s="176"/>
-      <c r="K2" s="176"/>
-      <c r="L2" s="176"/>
-      <c r="M2" s="176"/>
-      <c r="N2" s="176"/>
+      <c r="B2" s="177"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="177"/>
+      <c r="I2" s="177"/>
+      <c r="J2" s="177"/>
+      <c r="K2" s="177"/>
+      <c r="L2" s="177"/>
+      <c r="M2" s="177"/>
+      <c r="N2" s="177"/>
     </row>
     <row r="3" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A3" s="82"/>
@@ -6071,21 +6071,21 @@
       <c r="C3" s="192">
         <v>2022</v>
       </c>
-      <c r="D3" s="178"/>
-      <c r="E3" s="178"/>
-      <c r="F3" s="178"/>
-      <c r="G3" s="179">
+      <c r="D3" s="179"/>
+      <c r="E3" s="179"/>
+      <c r="F3" s="179"/>
+      <c r="G3" s="180">
         <v>2023</v>
       </c>
-      <c r="H3" s="180"/>
-      <c r="I3" s="180"/>
-      <c r="J3" s="181"/>
-      <c r="K3" s="179">
+      <c r="H3" s="181"/>
+      <c r="I3" s="181"/>
+      <c r="J3" s="182"/>
+      <c r="K3" s="180">
         <v>2024</v>
       </c>
-      <c r="L3" s="180"/>
-      <c r="M3" s="180"/>
-      <c r="N3" s="180"/>
+      <c r="L3" s="181"/>
+      <c r="M3" s="181"/>
+      <c r="N3" s="181"/>
     </row>
     <row r="4" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A4" s="84"/>
@@ -6590,22 +6590,22 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="182" t="s">
+      <c r="A16" s="175" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="182"/>
-      <c r="C16" s="182"/>
-      <c r="D16" s="182"/>
-      <c r="E16" s="182"/>
-      <c r="F16" s="182"/>
-      <c r="G16" s="182"/>
-      <c r="H16" s="182"/>
-      <c r="I16" s="182"/>
-      <c r="J16" s="182"/>
-      <c r="K16" s="182"/>
-      <c r="L16" s="182"/>
-      <c r="M16" s="182"/>
-      <c r="N16" s="182"/>
+      <c r="B16" s="175"/>
+      <c r="C16" s="175"/>
+      <c r="D16" s="175"/>
+      <c r="E16" s="175"/>
+      <c r="F16" s="175"/>
+      <c r="G16" s="175"/>
+      <c r="H16" s="175"/>
+      <c r="I16" s="175"/>
+      <c r="J16" s="175"/>
+      <c r="K16" s="175"/>
+      <c r="L16" s="175"/>
+      <c r="M16" s="175"/>
+      <c r="N16" s="175"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="104" t="s">
@@ -6654,62 +6654,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="175" t="s">
+      <c r="A1" s="176" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="175"/>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
-      <c r="G1" s="175"/>
-      <c r="H1" s="175"/>
-      <c r="I1" s="175"/>
-      <c r="J1" s="175"/>
-      <c r="K1" s="175"/>
-      <c r="L1" s="175"/>
-      <c r="M1" s="175"/>
-      <c r="N1" s="175"/>
+      <c r="B1" s="176"/>
+      <c r="C1" s="176"/>
+      <c r="D1" s="176"/>
+      <c r="E1" s="176"/>
+      <c r="F1" s="176"/>
+      <c r="G1" s="176"/>
+      <c r="H1" s="176"/>
+      <c r="I1" s="176"/>
+      <c r="J1" s="176"/>
+      <c r="K1" s="176"/>
+      <c r="L1" s="176"/>
+      <c r="M1" s="176"/>
+      <c r="N1" s="176"/>
     </row>
     <row r="2" spans="1:14" ht="13" x14ac:dyDescent="0.25">
-      <c r="A2" s="176" t="s">
+      <c r="A2" s="177" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="176"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="176"/>
-      <c r="F2" s="176"/>
-      <c r="G2" s="176"/>
-      <c r="H2" s="176"/>
-      <c r="I2" s="176"/>
-      <c r="J2" s="176"/>
-      <c r="K2" s="176"/>
-      <c r="L2" s="176"/>
-      <c r="M2" s="176"/>
-      <c r="N2" s="176"/>
+      <c r="B2" s="177"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="177"/>
+      <c r="I2" s="177"/>
+      <c r="J2" s="177"/>
+      <c r="K2" s="177"/>
+      <c r="L2" s="177"/>
+      <c r="M2" s="177"/>
+      <c r="N2" s="177"/>
     </row>
     <row r="3" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A3" s="82"/>
       <c r="B3" s="83"/>
-      <c r="C3" s="177">
+      <c r="C3" s="178">
         <v>2021</v>
       </c>
-      <c r="D3" s="178"/>
-      <c r="E3" s="178"/>
-      <c r="F3" s="178"/>
-      <c r="G3" s="179">
+      <c r="D3" s="179"/>
+      <c r="E3" s="179"/>
+      <c r="F3" s="179"/>
+      <c r="G3" s="180">
         <v>2022</v>
       </c>
-      <c r="H3" s="180"/>
-      <c r="I3" s="180"/>
-      <c r="J3" s="181"/>
-      <c r="K3" s="179">
+      <c r="H3" s="181"/>
+      <c r="I3" s="181"/>
+      <c r="J3" s="182"/>
+      <c r="K3" s="180">
         <v>2023</v>
       </c>
-      <c r="L3" s="180"/>
-      <c r="M3" s="180"/>
-      <c r="N3" s="180"/>
+      <c r="L3" s="181"/>
+      <c r="M3" s="181"/>
+      <c r="N3" s="181"/>
     </row>
     <row r="4" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A4" s="84"/>
@@ -7214,22 +7214,22 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="182" t="s">
+      <c r="A16" s="175" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="182"/>
-      <c r="C16" s="182"/>
-      <c r="D16" s="182"/>
-      <c r="E16" s="182"/>
-      <c r="F16" s="182"/>
-      <c r="G16" s="182"/>
-      <c r="H16" s="182"/>
-      <c r="I16" s="182"/>
-      <c r="J16" s="182"/>
-      <c r="K16" s="182"/>
-      <c r="L16" s="182"/>
-      <c r="M16" s="182"/>
-      <c r="N16" s="182"/>
+      <c r="B16" s="175"/>
+      <c r="C16" s="175"/>
+      <c r="D16" s="175"/>
+      <c r="E16" s="175"/>
+      <c r="F16" s="175"/>
+      <c r="G16" s="175"/>
+      <c r="H16" s="175"/>
+      <c r="I16" s="175"/>
+      <c r="J16" s="175"/>
+      <c r="K16" s="175"/>
+      <c r="L16" s="175"/>
+      <c r="M16" s="175"/>
+      <c r="N16" s="175"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="104" t="s">
@@ -7278,62 +7278,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="175" t="s">
+      <c r="A1" s="176" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="175"/>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
-      <c r="G1" s="175"/>
-      <c r="H1" s="175"/>
-      <c r="I1" s="175"/>
-      <c r="J1" s="175"/>
-      <c r="K1" s="175"/>
-      <c r="L1" s="175"/>
-      <c r="M1" s="175"/>
-      <c r="N1" s="175"/>
+      <c r="B1" s="176"/>
+      <c r="C1" s="176"/>
+      <c r="D1" s="176"/>
+      <c r="E1" s="176"/>
+      <c r="F1" s="176"/>
+      <c r="G1" s="176"/>
+      <c r="H1" s="176"/>
+      <c r="I1" s="176"/>
+      <c r="J1" s="176"/>
+      <c r="K1" s="176"/>
+      <c r="L1" s="176"/>
+      <c r="M1" s="176"/>
+      <c r="N1" s="176"/>
     </row>
     <row r="2" spans="1:14" ht="13" x14ac:dyDescent="0.25">
-      <c r="A2" s="176" t="s">
+      <c r="A2" s="177" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="176"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="176"/>
-      <c r="F2" s="176"/>
-      <c r="G2" s="176"/>
-      <c r="H2" s="176"/>
-      <c r="I2" s="176"/>
-      <c r="J2" s="176"/>
-      <c r="K2" s="176"/>
-      <c r="L2" s="176"/>
-      <c r="M2" s="176"/>
-      <c r="N2" s="176"/>
+      <c r="B2" s="177"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="177"/>
+      <c r="I2" s="177"/>
+      <c r="J2" s="177"/>
+      <c r="K2" s="177"/>
+      <c r="L2" s="177"/>
+      <c r="M2" s="177"/>
+      <c r="N2" s="177"/>
     </row>
     <row r="3" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A3" s="82"/>
       <c r="B3" s="83"/>
-      <c r="C3" s="177">
+      <c r="C3" s="178">
         <v>2021</v>
       </c>
-      <c r="D3" s="178"/>
-      <c r="E3" s="178"/>
-      <c r="F3" s="178"/>
-      <c r="G3" s="179">
+      <c r="D3" s="179"/>
+      <c r="E3" s="179"/>
+      <c r="F3" s="179"/>
+      <c r="G3" s="180">
         <v>2022</v>
       </c>
-      <c r="H3" s="180"/>
-      <c r="I3" s="180"/>
-      <c r="J3" s="181"/>
-      <c r="K3" s="179">
+      <c r="H3" s="181"/>
+      <c r="I3" s="181"/>
+      <c r="J3" s="182"/>
+      <c r="K3" s="180">
         <v>2023</v>
       </c>
-      <c r="L3" s="180"/>
-      <c r="M3" s="180"/>
-      <c r="N3" s="180"/>
+      <c r="L3" s="181"/>
+      <c r="M3" s="181"/>
+      <c r="N3" s="181"/>
     </row>
     <row r="4" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A4" s="84"/>
@@ -7838,22 +7838,22 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="182" t="s">
+      <c r="A16" s="175" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="182"/>
-      <c r="C16" s="182"/>
-      <c r="D16" s="182"/>
-      <c r="E16" s="182"/>
-      <c r="F16" s="182"/>
-      <c r="G16" s="182"/>
-      <c r="H16" s="182"/>
-      <c r="I16" s="182"/>
-      <c r="J16" s="182"/>
-      <c r="K16" s="182"/>
-      <c r="L16" s="182"/>
-      <c r="M16" s="182"/>
-      <c r="N16" s="182"/>
+      <c r="B16" s="175"/>
+      <c r="C16" s="175"/>
+      <c r="D16" s="175"/>
+      <c r="E16" s="175"/>
+      <c r="F16" s="175"/>
+      <c r="G16" s="175"/>
+      <c r="H16" s="175"/>
+      <c r="I16" s="175"/>
+      <c r="J16" s="175"/>
+      <c r="K16" s="175"/>
+      <c r="L16" s="175"/>
+      <c r="M16" s="175"/>
+      <c r="N16" s="175"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="104" t="s">
@@ -7902,62 +7902,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="175" t="s">
+      <c r="A1" s="176" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="175"/>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
-      <c r="G1" s="175"/>
-      <c r="H1" s="175"/>
-      <c r="I1" s="175"/>
-      <c r="J1" s="175"/>
-      <c r="K1" s="175"/>
-      <c r="L1" s="175"/>
-      <c r="M1" s="175"/>
-      <c r="N1" s="175"/>
+      <c r="B1" s="176"/>
+      <c r="C1" s="176"/>
+      <c r="D1" s="176"/>
+      <c r="E1" s="176"/>
+      <c r="F1" s="176"/>
+      <c r="G1" s="176"/>
+      <c r="H1" s="176"/>
+      <c r="I1" s="176"/>
+      <c r="J1" s="176"/>
+      <c r="K1" s="176"/>
+      <c r="L1" s="176"/>
+      <c r="M1" s="176"/>
+      <c r="N1" s="176"/>
     </row>
     <row r="2" spans="1:14" ht="13" x14ac:dyDescent="0.25">
-      <c r="A2" s="176" t="s">
+      <c r="A2" s="177" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="176"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="176"/>
-      <c r="F2" s="176"/>
-      <c r="G2" s="176"/>
-      <c r="H2" s="176"/>
-      <c r="I2" s="176"/>
-      <c r="J2" s="176"/>
-      <c r="K2" s="176"/>
-      <c r="L2" s="176"/>
-      <c r="M2" s="176"/>
-      <c r="N2" s="176"/>
+      <c r="B2" s="177"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="177"/>
+      <c r="I2" s="177"/>
+      <c r="J2" s="177"/>
+      <c r="K2" s="177"/>
+      <c r="L2" s="177"/>
+      <c r="M2" s="177"/>
+      <c r="N2" s="177"/>
     </row>
     <row r="3" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A3" s="82"/>
       <c r="B3" s="83"/>
-      <c r="C3" s="177">
+      <c r="C3" s="178">
         <v>2021</v>
       </c>
-      <c r="D3" s="178"/>
-      <c r="E3" s="178"/>
-      <c r="F3" s="178"/>
-      <c r="G3" s="179">
+      <c r="D3" s="179"/>
+      <c r="E3" s="179"/>
+      <c r="F3" s="179"/>
+      <c r="G3" s="180">
         <v>2022</v>
       </c>
-      <c r="H3" s="180"/>
-      <c r="I3" s="180"/>
-      <c r="J3" s="181"/>
-      <c r="K3" s="179">
+      <c r="H3" s="181"/>
+      <c r="I3" s="181"/>
+      <c r="J3" s="182"/>
+      <c r="K3" s="180">
         <v>2023</v>
       </c>
-      <c r="L3" s="180"/>
-      <c r="M3" s="180"/>
-      <c r="N3" s="180"/>
+      <c r="L3" s="181"/>
+      <c r="M3" s="181"/>
+      <c r="N3" s="181"/>
     </row>
     <row r="4" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A4" s="84"/>
@@ -8462,22 +8462,22 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="182" t="s">
+      <c r="A16" s="175" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="182"/>
-      <c r="C16" s="182"/>
-      <c r="D16" s="182"/>
-      <c r="E16" s="182"/>
-      <c r="F16" s="182"/>
-      <c r="G16" s="182"/>
-      <c r="H16" s="182"/>
-      <c r="I16" s="182"/>
-      <c r="J16" s="182"/>
-      <c r="K16" s="182"/>
-      <c r="L16" s="182"/>
-      <c r="M16" s="182"/>
-      <c r="N16" s="182"/>
+      <c r="B16" s="175"/>
+      <c r="C16" s="175"/>
+      <c r="D16" s="175"/>
+      <c r="E16" s="175"/>
+      <c r="F16" s="175"/>
+      <c r="G16" s="175"/>
+      <c r="H16" s="175"/>
+      <c r="I16" s="175"/>
+      <c r="J16" s="175"/>
+      <c r="K16" s="175"/>
+      <c r="L16" s="175"/>
+      <c r="M16" s="175"/>
+      <c r="N16" s="175"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="104" t="s">
@@ -8526,62 +8526,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="175" t="s">
+      <c r="A1" s="176" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="175"/>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
-      <c r="G1" s="175"/>
-      <c r="H1" s="175"/>
-      <c r="I1" s="175"/>
-      <c r="J1" s="175"/>
-      <c r="K1" s="175"/>
-      <c r="L1" s="175"/>
-      <c r="M1" s="175"/>
-      <c r="N1" s="175"/>
+      <c r="B1" s="176"/>
+      <c r="C1" s="176"/>
+      <c r="D1" s="176"/>
+      <c r="E1" s="176"/>
+      <c r="F1" s="176"/>
+      <c r="G1" s="176"/>
+      <c r="H1" s="176"/>
+      <c r="I1" s="176"/>
+      <c r="J1" s="176"/>
+      <c r="K1" s="176"/>
+      <c r="L1" s="176"/>
+      <c r="M1" s="176"/>
+      <c r="N1" s="176"/>
     </row>
     <row r="2" spans="1:14" ht="13" x14ac:dyDescent="0.25">
-      <c r="A2" s="176" t="s">
+      <c r="A2" s="177" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="176"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="176"/>
-      <c r="F2" s="176"/>
-      <c r="G2" s="176"/>
-      <c r="H2" s="176"/>
-      <c r="I2" s="176"/>
-      <c r="J2" s="176"/>
-      <c r="K2" s="176"/>
-      <c r="L2" s="176"/>
-      <c r="M2" s="176"/>
-      <c r="N2" s="176"/>
+      <c r="B2" s="177"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="177"/>
+      <c r="I2" s="177"/>
+      <c r="J2" s="177"/>
+      <c r="K2" s="177"/>
+      <c r="L2" s="177"/>
+      <c r="M2" s="177"/>
+      <c r="N2" s="177"/>
     </row>
     <row r="3" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A3" s="82"/>
       <c r="B3" s="83"/>
-      <c r="C3" s="177">
+      <c r="C3" s="178">
         <v>2021</v>
       </c>
-      <c r="D3" s="178"/>
-      <c r="E3" s="178"/>
-      <c r="F3" s="178"/>
-      <c r="G3" s="179">
+      <c r="D3" s="179"/>
+      <c r="E3" s="179"/>
+      <c r="F3" s="179"/>
+      <c r="G3" s="180">
         <v>2022</v>
       </c>
-      <c r="H3" s="180"/>
-      <c r="I3" s="180"/>
-      <c r="J3" s="181"/>
-      <c r="K3" s="179">
+      <c r="H3" s="181"/>
+      <c r="I3" s="181"/>
+      <c r="J3" s="182"/>
+      <c r="K3" s="180">
         <v>2023</v>
       </c>
-      <c r="L3" s="180"/>
-      <c r="M3" s="180"/>
-      <c r="N3" s="180"/>
+      <c r="L3" s="181"/>
+      <c r="M3" s="181"/>
+      <c r="N3" s="181"/>
     </row>
     <row r="4" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A4" s="84"/>
@@ -9086,22 +9086,22 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="182" t="s">
+      <c r="A16" s="175" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="182"/>
-      <c r="C16" s="182"/>
-      <c r="D16" s="182"/>
-      <c r="E16" s="182"/>
-      <c r="F16" s="182"/>
-      <c r="G16" s="182"/>
-      <c r="H16" s="182"/>
-      <c r="I16" s="182"/>
-      <c r="J16" s="182"/>
-      <c r="K16" s="182"/>
-      <c r="L16" s="182"/>
-      <c r="M16" s="182"/>
-      <c r="N16" s="182"/>
+      <c r="B16" s="175"/>
+      <c r="C16" s="175"/>
+      <c r="D16" s="175"/>
+      <c r="E16" s="175"/>
+      <c r="F16" s="175"/>
+      <c r="G16" s="175"/>
+      <c r="H16" s="175"/>
+      <c r="I16" s="175"/>
+      <c r="J16" s="175"/>
+      <c r="K16" s="175"/>
+      <c r="L16" s="175"/>
+      <c r="M16" s="175"/>
+      <c r="N16" s="175"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="104" t="s">
@@ -22632,62 +22632,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="175" t="s">
+      <c r="A1" s="176" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="175"/>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
-      <c r="G1" s="175"/>
-      <c r="H1" s="175"/>
-      <c r="I1" s="175"/>
-      <c r="J1" s="175"/>
-      <c r="K1" s="175"/>
-      <c r="L1" s="175"/>
-      <c r="M1" s="175"/>
-      <c r="N1" s="175"/>
+      <c r="B1" s="176"/>
+      <c r="C1" s="176"/>
+      <c r="D1" s="176"/>
+      <c r="E1" s="176"/>
+      <c r="F1" s="176"/>
+      <c r="G1" s="176"/>
+      <c r="H1" s="176"/>
+      <c r="I1" s="176"/>
+      <c r="J1" s="176"/>
+      <c r="K1" s="176"/>
+      <c r="L1" s="176"/>
+      <c r="M1" s="176"/>
+      <c r="N1" s="176"/>
     </row>
     <row r="2" spans="1:14" ht="13" x14ac:dyDescent="0.25">
-      <c r="A2" s="176" t="s">
+      <c r="A2" s="177" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="176"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="176"/>
-      <c r="F2" s="176"/>
-      <c r="G2" s="176"/>
-      <c r="H2" s="176"/>
-      <c r="I2" s="176"/>
-      <c r="J2" s="176"/>
-      <c r="K2" s="176"/>
-      <c r="L2" s="176"/>
-      <c r="M2" s="176"/>
-      <c r="N2" s="176"/>
+      <c r="B2" s="177"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="177"/>
+      <c r="I2" s="177"/>
+      <c r="J2" s="177"/>
+      <c r="K2" s="177"/>
+      <c r="L2" s="177"/>
+      <c r="M2" s="177"/>
+      <c r="N2" s="177"/>
     </row>
     <row r="3" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A3" s="82"/>
       <c r="B3" s="83"/>
-      <c r="C3" s="177">
+      <c r="C3" s="178">
         <v>2020</v>
       </c>
-      <c r="D3" s="178"/>
-      <c r="E3" s="178"/>
-      <c r="F3" s="178"/>
-      <c r="G3" s="179">
+      <c r="D3" s="179"/>
+      <c r="E3" s="179"/>
+      <c r="F3" s="179"/>
+      <c r="G3" s="180">
         <v>2021</v>
       </c>
-      <c r="H3" s="180"/>
-      <c r="I3" s="180"/>
-      <c r="J3" s="181"/>
-      <c r="K3" s="179">
+      <c r="H3" s="181"/>
+      <c r="I3" s="181"/>
+      <c r="J3" s="182"/>
+      <c r="K3" s="180">
         <v>2022</v>
       </c>
-      <c r="L3" s="180"/>
-      <c r="M3" s="180"/>
-      <c r="N3" s="180"/>
+      <c r="L3" s="181"/>
+      <c r="M3" s="181"/>
+      <c r="N3" s="181"/>
     </row>
     <row r="4" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A4" s="84"/>
@@ -23192,22 +23192,22 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="182" t="s">
+      <c r="A16" s="175" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="182"/>
-      <c r="C16" s="182"/>
-      <c r="D16" s="182"/>
-      <c r="E16" s="182"/>
-      <c r="F16" s="182"/>
-      <c r="G16" s="182"/>
-      <c r="H16" s="182"/>
-      <c r="I16" s="182"/>
-      <c r="J16" s="182"/>
-      <c r="K16" s="182"/>
-      <c r="L16" s="182"/>
-      <c r="M16" s="182"/>
-      <c r="N16" s="182"/>
+      <c r="B16" s="175"/>
+      <c r="C16" s="175"/>
+      <c r="D16" s="175"/>
+      <c r="E16" s="175"/>
+      <c r="F16" s="175"/>
+      <c r="G16" s="175"/>
+      <c r="H16" s="175"/>
+      <c r="I16" s="175"/>
+      <c r="J16" s="175"/>
+      <c r="K16" s="175"/>
+      <c r="L16" s="175"/>
+      <c r="M16" s="175"/>
+      <c r="N16" s="175"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="104" t="s">
@@ -23256,62 +23256,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="175" t="s">
+      <c r="A1" s="176" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="175"/>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
-      <c r="G1" s="175"/>
-      <c r="H1" s="175"/>
-      <c r="I1" s="175"/>
-      <c r="J1" s="175"/>
-      <c r="K1" s="175"/>
-      <c r="L1" s="175"/>
-      <c r="M1" s="175"/>
-      <c r="N1" s="175"/>
+      <c r="B1" s="176"/>
+      <c r="C1" s="176"/>
+      <c r="D1" s="176"/>
+      <c r="E1" s="176"/>
+      <c r="F1" s="176"/>
+      <c r="G1" s="176"/>
+      <c r="H1" s="176"/>
+      <c r="I1" s="176"/>
+      <c r="J1" s="176"/>
+      <c r="K1" s="176"/>
+      <c r="L1" s="176"/>
+      <c r="M1" s="176"/>
+      <c r="N1" s="176"/>
     </row>
     <row r="2" spans="1:14" ht="13" x14ac:dyDescent="0.25">
-      <c r="A2" s="176" t="s">
+      <c r="A2" s="177" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="176"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="176"/>
-      <c r="F2" s="176"/>
-      <c r="G2" s="176"/>
-      <c r="H2" s="176"/>
-      <c r="I2" s="176"/>
-      <c r="J2" s="176"/>
-      <c r="K2" s="176"/>
-      <c r="L2" s="176"/>
-      <c r="M2" s="176"/>
-      <c r="N2" s="176"/>
+      <c r="B2" s="177"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="177"/>
+      <c r="I2" s="177"/>
+      <c r="J2" s="177"/>
+      <c r="K2" s="177"/>
+      <c r="L2" s="177"/>
+      <c r="M2" s="177"/>
+      <c r="N2" s="177"/>
     </row>
     <row r="3" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A3" s="82"/>
       <c r="B3" s="83"/>
-      <c r="C3" s="177">
+      <c r="C3" s="178">
         <v>2020</v>
       </c>
-      <c r="D3" s="178"/>
-      <c r="E3" s="178"/>
-      <c r="F3" s="178"/>
-      <c r="G3" s="179">
+      <c r="D3" s="179"/>
+      <c r="E3" s="179"/>
+      <c r="F3" s="179"/>
+      <c r="G3" s="180">
         <v>2021</v>
       </c>
-      <c r="H3" s="180"/>
-      <c r="I3" s="180"/>
-      <c r="J3" s="181"/>
-      <c r="K3" s="179">
+      <c r="H3" s="181"/>
+      <c r="I3" s="181"/>
+      <c r="J3" s="182"/>
+      <c r="K3" s="180">
         <v>2022</v>
       </c>
-      <c r="L3" s="180"/>
-      <c r="M3" s="180"/>
-      <c r="N3" s="180"/>
+      <c r="L3" s="181"/>
+      <c r="M3" s="181"/>
+      <c r="N3" s="181"/>
     </row>
     <row r="4" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A4" s="84"/>
@@ -23816,22 +23816,22 @@
       </c>
     </row>
     <row r="16" spans="1:14" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="182" t="s">
+      <c r="A16" s="175" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="182"/>
-      <c r="C16" s="182"/>
-      <c r="D16" s="182"/>
-      <c r="E16" s="182"/>
-      <c r="F16" s="182"/>
-      <c r="G16" s="182"/>
-      <c r="H16" s="182"/>
-      <c r="I16" s="182"/>
-      <c r="J16" s="182"/>
-      <c r="K16" s="182"/>
-      <c r="L16" s="182"/>
-      <c r="M16" s="182"/>
-      <c r="N16" s="182"/>
+      <c r="B16" s="175"/>
+      <c r="C16" s="175"/>
+      <c r="D16" s="175"/>
+      <c r="E16" s="175"/>
+      <c r="F16" s="175"/>
+      <c r="G16" s="175"/>
+      <c r="H16" s="175"/>
+      <c r="I16" s="175"/>
+      <c r="J16" s="175"/>
+      <c r="K16" s="175"/>
+      <c r="L16" s="175"/>
+      <c r="M16" s="175"/>
+      <c r="N16" s="175"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="104" t="s">
@@ -23880,62 +23880,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="175" t="s">
+      <c r="A1" s="176" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="175"/>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
-      <c r="G1" s="175"/>
-      <c r="H1" s="175"/>
-      <c r="I1" s="175"/>
-      <c r="J1" s="175"/>
-      <c r="K1" s="175"/>
-      <c r="L1" s="175"/>
-      <c r="M1" s="175"/>
-      <c r="N1" s="175"/>
+      <c r="B1" s="176"/>
+      <c r="C1" s="176"/>
+      <c r="D1" s="176"/>
+      <c r="E1" s="176"/>
+      <c r="F1" s="176"/>
+      <c r="G1" s="176"/>
+      <c r="H1" s="176"/>
+      <c r="I1" s="176"/>
+      <c r="J1" s="176"/>
+      <c r="K1" s="176"/>
+      <c r="L1" s="176"/>
+      <c r="M1" s="176"/>
+      <c r="N1" s="176"/>
     </row>
     <row r="2" spans="1:14" ht="13" x14ac:dyDescent="0.25">
-      <c r="A2" s="176" t="s">
+      <c r="A2" s="177" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="176"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="176"/>
-      <c r="F2" s="176"/>
-      <c r="G2" s="176"/>
-      <c r="H2" s="176"/>
-      <c r="I2" s="176"/>
-      <c r="J2" s="176"/>
-      <c r="K2" s="176"/>
-      <c r="L2" s="176"/>
-      <c r="M2" s="176"/>
-      <c r="N2" s="176"/>
+      <c r="B2" s="177"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="177"/>
+      <c r="I2" s="177"/>
+      <c r="J2" s="177"/>
+      <c r="K2" s="177"/>
+      <c r="L2" s="177"/>
+      <c r="M2" s="177"/>
+      <c r="N2" s="177"/>
     </row>
     <row r="3" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A3" s="82"/>
       <c r="B3" s="83"/>
-      <c r="C3" s="177">
+      <c r="C3" s="178">
         <v>2020</v>
       </c>
-      <c r="D3" s="178"/>
-      <c r="E3" s="178"/>
-      <c r="F3" s="178"/>
-      <c r="G3" s="179">
+      <c r="D3" s="179"/>
+      <c r="E3" s="179"/>
+      <c r="F3" s="179"/>
+      <c r="G3" s="180">
         <v>2021</v>
       </c>
-      <c r="H3" s="180"/>
-      <c r="I3" s="180"/>
-      <c r="J3" s="181"/>
-      <c r="K3" s="179">
+      <c r="H3" s="181"/>
+      <c r="I3" s="181"/>
+      <c r="J3" s="182"/>
+      <c r="K3" s="180">
         <v>2022</v>
       </c>
-      <c r="L3" s="180"/>
-      <c r="M3" s="180"/>
-      <c r="N3" s="180"/>
+      <c r="L3" s="181"/>
+      <c r="M3" s="181"/>
+      <c r="N3" s="181"/>
     </row>
     <row r="4" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A4" s="84"/>
@@ -24440,22 +24440,22 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="182" t="s">
+      <c r="A16" s="175" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="182"/>
-      <c r="C16" s="182"/>
-      <c r="D16" s="182"/>
-      <c r="E16" s="182"/>
-      <c r="F16" s="182"/>
-      <c r="G16" s="182"/>
-      <c r="H16" s="182"/>
-      <c r="I16" s="182"/>
-      <c r="J16" s="182"/>
-      <c r="K16" s="182"/>
-      <c r="L16" s="182"/>
-      <c r="M16" s="182"/>
-      <c r="N16" s="182"/>
+      <c r="B16" s="175"/>
+      <c r="C16" s="175"/>
+      <c r="D16" s="175"/>
+      <c r="E16" s="175"/>
+      <c r="F16" s="175"/>
+      <c r="G16" s="175"/>
+      <c r="H16" s="175"/>
+      <c r="I16" s="175"/>
+      <c r="J16" s="175"/>
+      <c r="K16" s="175"/>
+      <c r="L16" s="175"/>
+      <c r="M16" s="175"/>
+      <c r="N16" s="175"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="104" t="s">
@@ -24494,7 +24494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{806A2F6E-FCA6-4C03-9E8F-930500601210}">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="C15" sqref="C15:N15"/>
     </sheetView>
   </sheetViews>
@@ -24504,40 +24504,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="175" t="s">
+      <c r="A1" s="176" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="175"/>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
-      <c r="G1" s="175"/>
-      <c r="H1" s="175"/>
-      <c r="I1" s="175"/>
-      <c r="J1" s="175"/>
-      <c r="K1" s="175"/>
-      <c r="L1" s="175"/>
-      <c r="M1" s="175"/>
-      <c r="N1" s="175"/>
+      <c r="B1" s="176"/>
+      <c r="C1" s="176"/>
+      <c r="D1" s="176"/>
+      <c r="E1" s="176"/>
+      <c r="F1" s="176"/>
+      <c r="G1" s="176"/>
+      <c r="H1" s="176"/>
+      <c r="I1" s="176"/>
+      <c r="J1" s="176"/>
+      <c r="K1" s="176"/>
+      <c r="L1" s="176"/>
+      <c r="M1" s="176"/>
+      <c r="N1" s="176"/>
     </row>
     <row r="2" spans="1:14" ht="13" x14ac:dyDescent="0.25">
-      <c r="A2" s="176" t="s">
+      <c r="A2" s="177" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="176"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="176"/>
-      <c r="F2" s="176"/>
-      <c r="G2" s="176"/>
-      <c r="H2" s="176"/>
-      <c r="I2" s="176"/>
-      <c r="J2" s="176"/>
-      <c r="K2" s="176"/>
-      <c r="L2" s="176"/>
-      <c r="M2" s="176"/>
-      <c r="N2" s="176"/>
+      <c r="B2" s="177"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="177"/>
+      <c r="I2" s="177"/>
+      <c r="J2" s="177"/>
+      <c r="K2" s="177"/>
+      <c r="L2" s="177"/>
+      <c r="M2" s="177"/>
+      <c r="N2" s="177"/>
     </row>
     <row r="3" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A3" s="82"/>
@@ -24548,18 +24548,18 @@
       <c r="D3" s="195"/>
       <c r="E3" s="195"/>
       <c r="F3" s="196"/>
-      <c r="G3" s="179">
+      <c r="G3" s="180">
         <v>2021</v>
       </c>
-      <c r="H3" s="180"/>
-      <c r="I3" s="180"/>
-      <c r="J3" s="181"/>
-      <c r="K3" s="179">
+      <c r="H3" s="181"/>
+      <c r="I3" s="181"/>
+      <c r="J3" s="182"/>
+      <c r="K3" s="180">
         <v>2022</v>
       </c>
-      <c r="L3" s="180"/>
-      <c r="M3" s="180"/>
-      <c r="N3" s="180"/>
+      <c r="L3" s="181"/>
+      <c r="M3" s="181"/>
+      <c r="N3" s="181"/>
     </row>
     <row r="4" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A4" s="84"/>
@@ -29046,64 +29046,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="175" t="s">
+      <c r="A1" s="176" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="175"/>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
-      <c r="G1" s="175"/>
-      <c r="H1" s="175"/>
-      <c r="I1" s="175"/>
-      <c r="J1" s="175"/>
-      <c r="K1" s="175"/>
-      <c r="L1" s="175"/>
-      <c r="M1" s="175"/>
-      <c r="N1" s="175"/>
+      <c r="B1" s="176"/>
+      <c r="C1" s="176"/>
+      <c r="D1" s="176"/>
+      <c r="E1" s="176"/>
+      <c r="F1" s="176"/>
+      <c r="G1" s="176"/>
+      <c r="H1" s="176"/>
+      <c r="I1" s="176"/>
+      <c r="J1" s="176"/>
+      <c r="K1" s="176"/>
+      <c r="L1" s="176"/>
+      <c r="M1" s="176"/>
+      <c r="N1" s="176"/>
     </row>
     <row r="2" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="176" t="s">
+      <c r="A2" s="177" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="176"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="176"/>
-      <c r="F2" s="176"/>
-      <c r="G2" s="176"/>
-      <c r="H2" s="176"/>
-      <c r="I2" s="176"/>
-      <c r="J2" s="176"/>
-      <c r="K2" s="176"/>
-      <c r="L2" s="176"/>
-      <c r="M2" s="176"/>
-      <c r="N2" s="176"/>
+      <c r="B2" s="177"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="177"/>
+      <c r="I2" s="177"/>
+      <c r="J2" s="177"/>
+      <c r="K2" s="177"/>
+      <c r="L2" s="177"/>
+      <c r="M2" s="177"/>
+      <c r="N2" s="177"/>
     </row>
     <row r="3" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="82"/>
       <c r="B3" s="83"/>
-      <c r="C3" s="177">
+      <c r="C3" s="178">
         <v>2025</v>
       </c>
-      <c r="D3" s="178"/>
-      <c r="E3" s="178"/>
-      <c r="F3" s="178"/>
-      <c r="G3" s="179">
+      <c r="D3" s="179"/>
+      <c r="E3" s="179"/>
+      <c r="F3" s="179"/>
+      <c r="G3" s="180">
         <f>C3+1</f>
         <v>2026</v>
       </c>
-      <c r="H3" s="180"/>
-      <c r="I3" s="180"/>
-      <c r="J3" s="181"/>
-      <c r="K3" s="179">
+      <c r="H3" s="181"/>
+      <c r="I3" s="181"/>
+      <c r="J3" s="182"/>
+      <c r="K3" s="180">
         <f>G3+1</f>
         <v>2027</v>
       </c>
-      <c r="L3" s="180"/>
-      <c r="M3" s="180"/>
-      <c r="N3" s="180"/>
+      <c r="L3" s="181"/>
+      <c r="M3" s="181"/>
+      <c r="N3" s="181"/>
     </row>
     <row r="4" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="84"/>
@@ -29608,22 +29608,22 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="182" t="s">
+      <c r="A16" s="175" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="182"/>
-      <c r="C16" s="182"/>
-      <c r="D16" s="182"/>
-      <c r="E16" s="182"/>
-      <c r="F16" s="182"/>
-      <c r="G16" s="182"/>
-      <c r="H16" s="182"/>
-      <c r="I16" s="182"/>
-      <c r="J16" s="182"/>
-      <c r="K16" s="182"/>
-      <c r="L16" s="182"/>
-      <c r="M16" s="182"/>
-      <c r="N16" s="182"/>
+      <c r="B16" s="175"/>
+      <c r="C16" s="175"/>
+      <c r="D16" s="175"/>
+      <c r="E16" s="175"/>
+      <c r="F16" s="175"/>
+      <c r="G16" s="175"/>
+      <c r="H16" s="175"/>
+      <c r="I16" s="175"/>
+      <c r="J16" s="175"/>
+      <c r="K16" s="175"/>
+      <c r="L16" s="175"/>
+      <c r="M16" s="175"/>
+      <c r="N16" s="175"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="104" t="s">
@@ -38824,64 +38824,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="175" t="s">
+      <c r="A1" s="176" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="175"/>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
-      <c r="G1" s="175"/>
-      <c r="H1" s="175"/>
-      <c r="I1" s="175"/>
-      <c r="J1" s="175"/>
-      <c r="K1" s="175"/>
-      <c r="L1" s="175"/>
-      <c r="M1" s="175"/>
-      <c r="N1" s="175"/>
+      <c r="B1" s="176"/>
+      <c r="C1" s="176"/>
+      <c r="D1" s="176"/>
+      <c r="E1" s="176"/>
+      <c r="F1" s="176"/>
+      <c r="G1" s="176"/>
+      <c r="H1" s="176"/>
+      <c r="I1" s="176"/>
+      <c r="J1" s="176"/>
+      <c r="K1" s="176"/>
+      <c r="L1" s="176"/>
+      <c r="M1" s="176"/>
+      <c r="N1" s="176"/>
     </row>
     <row r="2" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="176" t="s">
+      <c r="A2" s="177" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="176"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="176"/>
-      <c r="F2" s="176"/>
-      <c r="G2" s="176"/>
-      <c r="H2" s="176"/>
-      <c r="I2" s="176"/>
-      <c r="J2" s="176"/>
-      <c r="K2" s="176"/>
-      <c r="L2" s="176"/>
-      <c r="M2" s="176"/>
-      <c r="N2" s="176"/>
+      <c r="B2" s="177"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="177"/>
+      <c r="I2" s="177"/>
+      <c r="J2" s="177"/>
+      <c r="K2" s="177"/>
+      <c r="L2" s="177"/>
+      <c r="M2" s="177"/>
+      <c r="N2" s="177"/>
     </row>
     <row r="3" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="82"/>
       <c r="B3" s="83"/>
-      <c r="C3" s="177">
+      <c r="C3" s="178">
         <v>2024</v>
       </c>
-      <c r="D3" s="178"/>
-      <c r="E3" s="178"/>
-      <c r="F3" s="178"/>
-      <c r="G3" s="179">
+      <c r="D3" s="179"/>
+      <c r="E3" s="179"/>
+      <c r="F3" s="179"/>
+      <c r="G3" s="180">
         <f>C3+1</f>
         <v>2025</v>
       </c>
-      <c r="H3" s="180"/>
-      <c r="I3" s="180"/>
-      <c r="J3" s="181"/>
-      <c r="K3" s="179">
+      <c r="H3" s="181"/>
+      <c r="I3" s="181"/>
+      <c r="J3" s="182"/>
+      <c r="K3" s="180">
         <f>G3+1</f>
         <v>2026</v>
       </c>
-      <c r="L3" s="180"/>
-      <c r="M3" s="180"/>
-      <c r="N3" s="180"/>
+      <c r="L3" s="181"/>
+      <c r="M3" s="181"/>
+      <c r="N3" s="181"/>
     </row>
     <row r="4" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="84"/>
@@ -39386,22 +39386,22 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="182" t="s">
+      <c r="A16" s="175" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="182"/>
-      <c r="C16" s="182"/>
-      <c r="D16" s="182"/>
-      <c r="E16" s="182"/>
-      <c r="F16" s="182"/>
-      <c r="G16" s="182"/>
-      <c r="H16" s="182"/>
-      <c r="I16" s="182"/>
-      <c r="J16" s="182"/>
-      <c r="K16" s="182"/>
-      <c r="L16" s="182"/>
-      <c r="M16" s="182"/>
-      <c r="N16" s="182"/>
+      <c r="B16" s="175"/>
+      <c r="C16" s="175"/>
+      <c r="D16" s="175"/>
+      <c r="E16" s="175"/>
+      <c r="F16" s="175"/>
+      <c r="G16" s="175"/>
+      <c r="H16" s="175"/>
+      <c r="I16" s="175"/>
+      <c r="J16" s="175"/>
+      <c r="K16" s="175"/>
+      <c r="L16" s="175"/>
+      <c r="M16" s="175"/>
+      <c r="N16" s="175"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="104" t="s">
@@ -47185,7 +47185,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EEADAE7-5144-4852-BCE3-2541E80B3DF7}">
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="U28" sqref="U28"/>
     </sheetView>
   </sheetViews>
@@ -50513,64 +50513,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="175" t="s">
+      <c r="A1" s="176" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="175"/>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
-      <c r="G1" s="175"/>
-      <c r="H1" s="175"/>
-      <c r="I1" s="175"/>
-      <c r="J1" s="175"/>
-      <c r="K1" s="175"/>
-      <c r="L1" s="175"/>
-      <c r="M1" s="175"/>
-      <c r="N1" s="175"/>
+      <c r="B1" s="176"/>
+      <c r="C1" s="176"/>
+      <c r="D1" s="176"/>
+      <c r="E1" s="176"/>
+      <c r="F1" s="176"/>
+      <c r="G1" s="176"/>
+      <c r="H1" s="176"/>
+      <c r="I1" s="176"/>
+      <c r="J1" s="176"/>
+      <c r="K1" s="176"/>
+      <c r="L1" s="176"/>
+      <c r="M1" s="176"/>
+      <c r="N1" s="176"/>
     </row>
     <row r="2" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="176" t="s">
+      <c r="A2" s="177" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="176"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="176"/>
-      <c r="F2" s="176"/>
-      <c r="G2" s="176"/>
-      <c r="H2" s="176"/>
-      <c r="I2" s="176"/>
-      <c r="J2" s="176"/>
-      <c r="K2" s="176"/>
-      <c r="L2" s="176"/>
-      <c r="M2" s="176"/>
-      <c r="N2" s="176"/>
+      <c r="B2" s="177"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="177"/>
+      <c r="I2" s="177"/>
+      <c r="J2" s="177"/>
+      <c r="K2" s="177"/>
+      <c r="L2" s="177"/>
+      <c r="M2" s="177"/>
+      <c r="N2" s="177"/>
     </row>
     <row r="3" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="82"/>
       <c r="B3" s="83"/>
-      <c r="C3" s="177">
+      <c r="C3" s="178">
         <v>2024</v>
       </c>
-      <c r="D3" s="178"/>
-      <c r="E3" s="178"/>
-      <c r="F3" s="178"/>
-      <c r="G3" s="179">
+      <c r="D3" s="179"/>
+      <c r="E3" s="179"/>
+      <c r="F3" s="179"/>
+      <c r="G3" s="180">
         <f>C3+1</f>
         <v>2025</v>
       </c>
-      <c r="H3" s="180"/>
-      <c r="I3" s="180"/>
-      <c r="J3" s="181"/>
-      <c r="K3" s="179">
+      <c r="H3" s="181"/>
+      <c r="I3" s="181"/>
+      <c r="J3" s="182"/>
+      <c r="K3" s="180">
         <f>G3+1</f>
         <v>2026</v>
       </c>
-      <c r="L3" s="180"/>
-      <c r="M3" s="180"/>
-      <c r="N3" s="180"/>
+      <c r="L3" s="181"/>
+      <c r="M3" s="181"/>
+      <c r="N3" s="181"/>
     </row>
     <row r="4" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="84"/>
@@ -51075,22 +51075,22 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="182" t="s">
+      <c r="A16" s="175" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="182"/>
-      <c r="C16" s="182"/>
-      <c r="D16" s="182"/>
-      <c r="E16" s="182"/>
-      <c r="F16" s="182"/>
-      <c r="G16" s="182"/>
-      <c r="H16" s="182"/>
-      <c r="I16" s="182"/>
-      <c r="J16" s="182"/>
-      <c r="K16" s="182"/>
-      <c r="L16" s="182"/>
-      <c r="M16" s="182"/>
-      <c r="N16" s="182"/>
+      <c r="B16" s="175"/>
+      <c r="C16" s="175"/>
+      <c r="D16" s="175"/>
+      <c r="E16" s="175"/>
+      <c r="F16" s="175"/>
+      <c r="G16" s="175"/>
+      <c r="H16" s="175"/>
+      <c r="I16" s="175"/>
+      <c r="J16" s="175"/>
+      <c r="K16" s="175"/>
+      <c r="L16" s="175"/>
+      <c r="M16" s="175"/>
+      <c r="N16" s="175"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="104" t="s">
@@ -54436,8 +54436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C97EC740-24D9-4B89-9FDA-03564B892489}">
   <dimension ref="A1:AI40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32:R32"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -55728,8 +55728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C841121-D157-4629-B6F3-7B465A3856AD}">
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32:R32"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="T18" sqref="T18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -56235,7 +56235,7 @@
         <v>0.55832629889312102</v>
       </c>
       <c r="N18" s="138">
-        <v>-0.9202615158156533</v>
+        <v>-0.92026151581565296</v>
       </c>
       <c r="O18" s="137">
         <v>0.8502338137106733</v>
@@ -56839,22 +56839,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="175" t="s">
+      <c r="A1" s="176" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="175"/>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
-      <c r="G1" s="175"/>
-      <c r="H1" s="175"/>
-      <c r="I1" s="175"/>
-      <c r="J1" s="175"/>
-      <c r="K1" s="175"/>
-      <c r="L1" s="175"/>
-      <c r="M1" s="175"/>
-      <c r="N1" s="175"/>
+      <c r="B1" s="176"/>
+      <c r="C1" s="176"/>
+      <c r="D1" s="176"/>
+      <c r="E1" s="176"/>
+      <c r="F1" s="176"/>
+      <c r="G1" s="176"/>
+      <c r="H1" s="176"/>
+      <c r="I1" s="176"/>
+      <c r="J1" s="176"/>
+      <c r="K1" s="176"/>
+      <c r="L1" s="176"/>
+      <c r="M1" s="176"/>
+      <c r="N1" s="176"/>
     </row>
     <row r="2" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="154" t="s">
@@ -56875,46 +56875,46 @@
       <c r="N2" s="155"/>
     </row>
     <row r="3" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="176" t="s">
+      <c r="A3" s="177" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="176"/>
-      <c r="C3" s="176"/>
-      <c r="D3" s="176"/>
-      <c r="E3" s="176"/>
-      <c r="F3" s="176"/>
-      <c r="G3" s="176"/>
-      <c r="H3" s="176"/>
-      <c r="I3" s="176"/>
-      <c r="J3" s="176"/>
-      <c r="K3" s="176"/>
-      <c r="L3" s="176"/>
-      <c r="M3" s="176"/>
-      <c r="N3" s="176"/>
+      <c r="B3" s="177"/>
+      <c r="C3" s="177"/>
+      <c r="D3" s="177"/>
+      <c r="E3" s="177"/>
+      <c r="F3" s="177"/>
+      <c r="G3" s="177"/>
+      <c r="H3" s="177"/>
+      <c r="I3" s="177"/>
+      <c r="J3" s="177"/>
+      <c r="K3" s="177"/>
+      <c r="L3" s="177"/>
+      <c r="M3" s="177"/>
+      <c r="N3" s="177"/>
     </row>
     <row r="4" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="82"/>
       <c r="B4" s="83"/>
-      <c r="C4" s="177">
+      <c r="C4" s="178">
         <v>2024</v>
       </c>
-      <c r="D4" s="178"/>
-      <c r="E4" s="178"/>
-      <c r="F4" s="178"/>
-      <c r="G4" s="179">
+      <c r="D4" s="179"/>
+      <c r="E4" s="179"/>
+      <c r="F4" s="179"/>
+      <c r="G4" s="180">
         <f>C4+1</f>
         <v>2025</v>
       </c>
-      <c r="H4" s="180"/>
-      <c r="I4" s="180"/>
-      <c r="J4" s="181"/>
-      <c r="K4" s="179">
+      <c r="H4" s="181"/>
+      <c r="I4" s="181"/>
+      <c r="J4" s="182"/>
+      <c r="K4" s="180">
         <f>G4+1</f>
         <v>2026</v>
       </c>
-      <c r="L4" s="180"/>
-      <c r="M4" s="180"/>
-      <c r="N4" s="180"/>
+      <c r="L4" s="181"/>
+      <c r="M4" s="181"/>
+      <c r="N4" s="181"/>
     </row>
     <row r="5" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="84"/>
@@ -57425,46 +57425,46 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19" s="176" t="s">
+      <c r="A19" s="177" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="176"/>
-      <c r="C19" s="176"/>
-      <c r="D19" s="176"/>
-      <c r="E19" s="176"/>
-      <c r="F19" s="176"/>
-      <c r="G19" s="176"/>
-      <c r="H19" s="176"/>
-      <c r="I19" s="176"/>
-      <c r="J19" s="176"/>
-      <c r="K19" s="176"/>
-      <c r="L19" s="176"/>
-      <c r="M19" s="176"/>
-      <c r="N19" s="176"/>
+      <c r="B19" s="177"/>
+      <c r="C19" s="177"/>
+      <c r="D19" s="177"/>
+      <c r="E19" s="177"/>
+      <c r="F19" s="177"/>
+      <c r="G19" s="177"/>
+      <c r="H19" s="177"/>
+      <c r="I19" s="177"/>
+      <c r="J19" s="177"/>
+      <c r="K19" s="177"/>
+      <c r="L19" s="177"/>
+      <c r="M19" s="177"/>
+      <c r="N19" s="177"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="82"/>
       <c r="B20" s="83"/>
-      <c r="C20" s="177">
+      <c r="C20" s="178">
         <v>2024</v>
       </c>
-      <c r="D20" s="178"/>
-      <c r="E20" s="178"/>
-      <c r="F20" s="178"/>
-      <c r="G20" s="179">
+      <c r="D20" s="179"/>
+      <c r="E20" s="179"/>
+      <c r="F20" s="179"/>
+      <c r="G20" s="180">
         <f>C20+1</f>
         <v>2025</v>
       </c>
-      <c r="H20" s="180"/>
-      <c r="I20" s="180"/>
-      <c r="J20" s="181"/>
-      <c r="K20" s="179">
+      <c r="H20" s="181"/>
+      <c r="I20" s="181"/>
+      <c r="J20" s="182"/>
+      <c r="K20" s="180">
         <f>G20+1</f>
         <v>2026</v>
       </c>
-      <c r="L20" s="180"/>
-      <c r="M20" s="180"/>
-      <c r="N20" s="180"/>
+      <c r="L20" s="181"/>
+      <c r="M20" s="181"/>
+      <c r="N20" s="181"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="84"/>
@@ -57969,22 +57969,22 @@
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A33" s="182" t="s">
+      <c r="A33" s="175" t="s">
         <v>35</v>
       </c>
-      <c r="B33" s="182"/>
-      <c r="C33" s="182"/>
-      <c r="D33" s="182"/>
-      <c r="E33" s="182"/>
-      <c r="F33" s="182"/>
-      <c r="G33" s="182"/>
-      <c r="H33" s="182"/>
-      <c r="I33" s="182"/>
-      <c r="J33" s="182"/>
-      <c r="K33" s="182"/>
-      <c r="L33" s="182"/>
-      <c r="M33" s="182"/>
-      <c r="N33" s="182"/>
+      <c r="B33" s="175"/>
+      <c r="C33" s="175"/>
+      <c r="D33" s="175"/>
+      <c r="E33" s="175"/>
+      <c r="F33" s="175"/>
+      <c r="G33" s="175"/>
+      <c r="H33" s="175"/>
+      <c r="I33" s="175"/>
+      <c r="J33" s="175"/>
+      <c r="K33" s="175"/>
+      <c r="L33" s="175"/>
+      <c r="M33" s="175"/>
+      <c r="N33" s="175"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="104" t="s">
@@ -59910,12 +59910,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -59924,7 +59918,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100812A74FD0E0FD24B98E1BEFEEAEBFBDC" ma:contentTypeVersion="1" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="e1179fb03807e0db7f6fa766afcec06c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="45c57730-1a3d-4221-8b68-a26bacc245af" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="62da1e3614d9744e292be4b221a77d50" ns2:_="">
     <xsd:import namespace="45c57730-1a3d-4221-8b68-a26bacc245af"/>
@@ -60064,23 +60058,13 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA671E6F-F4B0-4949-873C-0E02EFE38C22}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="45c57730-1a3d-4221-8b68-a26bacc245af"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{592A31E8-CC0D-4A6E-A1EB-0EEA4A023AC3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -60088,7 +60072,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA4612ED-F8A4-4C2B-BBDD-36465B9B242C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -60104,4 +60088,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA671E6F-F4B0-4949-873C-0E02EFE38C22}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="45c57730-1a3d-4221-8b68-a26bacc245af"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>